<commit_message>
fix missing area in reference file
</commit_message>
<xml_diff>
--- a/test/ReferenceExcelFiles/Bob - gem_MKI_per_m2.xlsx
+++ b/test/ReferenceExcelFiles/Bob - gem_MKI_per_m2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://365tno-my.sharepoint.com/personal/diana_godoibizarro_tno_nl/Documents/BIM Bots/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vijj\Java\bim_workspace\BouwBesluitMaterials\test\ReferenceExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="983" documentId="8_{F6989E00-C8BF-4C7E-87D2-690DDBE64F21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{9A0D577F-DB42-4690-A245-3A258DDB3E4B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D81F8668-FDAB-4AD7-8B91-546BF1654982}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="330" windowWidth="20370" windowHeight="7815" tabRatio="845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-6480" windowWidth="29040" windowHeight="15840" tabRatio="845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM rijtjeswoning" sheetId="3" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1507,39 +1508,39 @@
   <sheetPr codeName="Blad4"/>
   <dimension ref="A1:Y43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E12" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.140625" style="17" customWidth="1"/>
-    <col min="2" max="4" width="33.5703125" style="17" customWidth="1"/>
-    <col min="5" max="5" width="32.85546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="7" customWidth="1"/>
-    <col min="7" max="8" width="19.85546875" style="7" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" style="74" customWidth="1"/>
-    <col min="10" max="11" width="19.85546875" style="7" customWidth="1"/>
-    <col min="12" max="12" width="19.85546875" style="74" customWidth="1"/>
-    <col min="13" max="15" width="19.85546875" style="7" customWidth="1"/>
-    <col min="16" max="16" width="19.85546875" style="74" customWidth="1"/>
-    <col min="17" max="17" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.7109375" style="9" customWidth="1"/>
-    <col min="20" max="20" width="56.140625" style="83" customWidth="1"/>
-    <col min="21" max="22" width="9.140625" style="71"/>
-    <col min="23" max="23" width="7.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="86.42578125" style="23" customWidth="1"/>
+    <col min="1" max="1" width="27.1796875" style="17" customWidth="1"/>
+    <col min="2" max="4" width="33.54296875" style="17" customWidth="1"/>
+    <col min="5" max="5" width="32.81640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="13.81640625" style="7" customWidth="1"/>
+    <col min="7" max="8" width="19.81640625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="19.81640625" style="74" customWidth="1"/>
+    <col min="10" max="11" width="19.81640625" style="7" customWidth="1"/>
+    <col min="12" max="12" width="19.81640625" style="74" customWidth="1"/>
+    <col min="13" max="15" width="19.81640625" style="7" customWidth="1"/>
+    <col min="16" max="16" width="19.81640625" style="74" customWidth="1"/>
+    <col min="17" max="17" width="10.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.7265625" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.7265625" style="9" customWidth="1"/>
+    <col min="20" max="20" width="56.1796875" style="83" customWidth="1"/>
+    <col min="21" max="22" width="9.1796875" style="71"/>
+    <col min="23" max="23" width="7.7265625" style="23" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.1796875" style="23" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="86.453125" style="23" customWidth="1"/>
     <col min="26" max="26" width="24" style="23" customWidth="1"/>
-    <col min="27" max="27" width="20.7109375" style="23" customWidth="1"/>
-    <col min="28" max="16384" width="9.140625" style="23"/>
+    <col min="27" max="27" width="20.7265625" style="23" customWidth="1"/>
+    <col min="28" max="16384" width="9.1796875" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="58" t="s">
         <v>22</v>
       </c>
@@ -1609,7 +1610,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="89" t="s">
         <v>25</v>
       </c>
@@ -1622,9 +1623,9 @@
       <c r="D2" s="92" t="s">
         <v>99</v>
       </c>
-      <c r="E2" s="93">
+      <c r="E2" s="93" t="e">
         <f>VLOOKUP(F2,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>1</v>
+        <v>#N/A</v>
       </c>
       <c r="F2" s="94" t="s">
         <v>3</v>
@@ -1691,7 +1692,7 @@
         <v>223.213536</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="59" t="s">
         <v>25</v>
       </c>
@@ -1704,9 +1705,9 @@
       <c r="D3" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="E3" s="56">
+      <c r="E3" s="56" t="e">
         <f>VLOOKUP(F3,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>9</v>
+        <v>#N/A</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>26</v>
@@ -1771,7 +1772,7 @@
         <v>85.850396099999969</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="59" t="s">
         <v>25</v>
       </c>
@@ -1784,9 +1785,9 @@
       <c r="D4" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="E4" s="56" t="str">
+      <c r="E4" s="56" t="e">
         <f>VLOOKUP(F4,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>71</v>
+        <v>#N/A</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>20</v>
@@ -1851,7 +1852,7 @@
         <v>434.52611999999993</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="59" t="s">
         <v>4</v>
       </c>
@@ -1864,9 +1865,9 @@
       <c r="D5" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="E5" s="56" t="str">
+      <c r="E5" s="56" t="e">
         <f>VLOOKUP(F5,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>71</v>
+        <v>#N/A</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>20</v>
@@ -1923,7 +1924,7 @@
         <v>926.20080000000007</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="59" t="s">
         <v>4</v>
       </c>
@@ -1936,9 +1937,9 @@
       <c r="D6" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="56">
+      <c r="E6" s="56" t="e">
         <f>VLOOKUP(F6,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>9</v>
+        <v>#N/A</v>
       </c>
       <c r="F6" s="14" t="s">
         <v>26</v>
@@ -1994,7 +1995,7 @@
         <v>192.62291999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="59" t="s">
         <v>4</v>
       </c>
@@ -2007,9 +2008,9 @@
       <c r="D7" s="48" t="s">
         <v>94</v>
       </c>
-      <c r="E7" s="56" t="str">
+      <c r="E7" s="56" t="e">
         <f>VLOOKUP(F7,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>57</v>
+        <v>#N/A</v>
       </c>
       <c r="F7" s="14" t="s">
         <v>113</v>
@@ -2061,11 +2062,11 @@
         <v>1.1906666666666665</v>
       </c>
       <c r="X7" s="60">
-        <f>U7*Q7</f>
+        <f t="shared" ref="X7:X20" si="1">U7*Q7</f>
         <v>103.58799999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="24" t="s">
         <v>5</v>
       </c>
@@ -2078,9 +2079,9 @@
       <c r="D8" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="E8" s="56">
+      <c r="E8" s="56" t="e">
         <f>VLOOKUP(F8,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>2</v>
+        <v>#N/A</v>
       </c>
       <c r="F8" s="14" t="s">
         <v>2</v>
@@ -2133,11 +2134,11 @@
         <v>0.33655172413793105</v>
       </c>
       <c r="X8" s="60">
-        <f>U8*Q8</f>
+        <f t="shared" si="1"/>
         <v>29.28</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="58" t="s">
         <v>5</v>
       </c>
@@ -2150,9 +2151,9 @@
       <c r="D9" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="56">
+      <c r="E9" s="56" t="e">
         <f>VLOOKUP(F9,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>2</v>
+        <v>#N/A</v>
       </c>
       <c r="F9" s="14" t="s">
         <v>2</v>
@@ -2181,7 +2182,7 @@
       </c>
       <c r="N9" s="75"/>
       <c r="O9" s="75">
-        <f>Q9/P9</f>
+        <f t="shared" ref="O9:O19" si="2">Q9/P9</f>
         <v>3.0150000000000001</v>
       </c>
       <c r="P9" s="64">
@@ -2213,11 +2214,11 @@
         <v>0.63418965517241377</v>
       </c>
       <c r="X9" s="60">
-        <f>U9*Q9</f>
+        <f t="shared" si="1"/>
         <v>55.174500000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="59" t="s">
         <v>85</v>
       </c>
@@ -2230,9 +2231,9 @@
       <c r="D10" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="E10" s="56">
+      <c r="E10" s="56" t="e">
         <f>VLOOKUP(F10,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>1</v>
+        <v>#N/A</v>
       </c>
       <c r="F10" s="14" t="s">
         <v>3</v>
@@ -2257,7 +2258,7 @@
         <v>151</v>
       </c>
       <c r="O10" s="75">
-        <f>Q10/P10</f>
+        <f t="shared" si="2"/>
         <v>9.5299999999999994</v>
       </c>
       <c r="P10" s="64">
@@ -2289,11 +2290,11 @@
         <v>8.715020689655173</v>
       </c>
       <c r="X10" s="60">
-        <f>U10*Q10</f>
+        <f t="shared" si="1"/>
         <v>758.20680000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="59" t="s">
         <v>85</v>
       </c>
@@ -2306,9 +2307,9 @@
       <c r="D11" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="E11" s="56">
+      <c r="E11" s="56" t="e">
         <f>VLOOKUP(F11,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>3</v>
+        <v>#N/A</v>
       </c>
       <c r="F11" s="14" t="s">
         <v>7</v>
@@ -2334,7 +2335,7 @@
       </c>
       <c r="N11" s="75"/>
       <c r="O11" s="75">
-        <f>Q11/P11</f>
+        <f t="shared" si="2"/>
         <v>9.5299999999999994</v>
       </c>
       <c r="P11" s="64">
@@ -2363,11 +2364,11 @@
         <v>5.4025241379310351</v>
       </c>
       <c r="X11" s="60">
-        <f>U11*Q11</f>
+        <f t="shared" si="1"/>
         <v>470.01960000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="24" t="s">
         <v>6</v>
       </c>
@@ -2380,9 +2381,9 @@
       <c r="D12" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="56">
+      <c r="E12" s="56" t="e">
         <f>VLOOKUP(F12,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>5</v>
+        <v>#N/A</v>
       </c>
       <c r="F12" s="14" t="s">
         <v>8</v>
@@ -2405,7 +2406,7 @@
       </c>
       <c r="N12" s="75"/>
       <c r="O12" s="75">
-        <f>Q12/P12</f>
+        <f t="shared" si="2"/>
         <v>0.41453999999999991</v>
       </c>
       <c r="P12" s="64">
@@ -2437,11 +2438,11 @@
         <v>4.7028848275862067E-2</v>
       </c>
       <c r="X12" s="60">
-        <f>U12*Q12</f>
+        <f t="shared" si="1"/>
         <v>4.0915097999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="59" t="s">
         <v>84</v>
       </c>
@@ -2454,9 +2455,9 @@
       <c r="D13" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="56">
+      <c r="E13" s="56" t="e">
         <f>VLOOKUP(F13,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>3</v>
+        <v>#N/A</v>
       </c>
       <c r="F13" s="14" t="s">
         <v>7</v>
@@ -2477,7 +2478,7 @@
       </c>
       <c r="N13" s="75"/>
       <c r="O13" s="75">
-        <f>Q13/P13</f>
+        <f t="shared" si="2"/>
         <v>0.39166666666666666</v>
       </c>
       <c r="P13" s="64">
@@ -2506,11 +2507,11 @@
         <v>0.2220344827586207</v>
       </c>
       <c r="X13" s="60">
-        <f>U13*Q13</f>
+        <f t="shared" si="1"/>
         <v>19.317</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="59" t="s">
         <v>84</v>
       </c>
@@ -2523,9 +2524,9 @@
       <c r="D14" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="E14" s="56">
+      <c r="E14" s="56" t="e">
         <f>VLOOKUP(F14,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>16</v>
+        <v>#N/A</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>109</v>
@@ -2550,7 +2551,7 @@
       </c>
       <c r="N14" s="75"/>
       <c r="O14" s="75">
-        <f>Q14/P14</f>
+        <f t="shared" si="2"/>
         <v>1.1749999999999998</v>
       </c>
       <c r="P14" s="64">
@@ -2582,11 +2583,11 @@
         <v>0.24384626436781603</v>
       </c>
       <c r="X14" s="60">
-        <f>U14*Q14</f>
+        <f t="shared" si="1"/>
         <v>21.214624999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="59" t="s">
         <v>84</v>
       </c>
@@ -2599,9 +2600,9 @@
       <c r="D15" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="E15" s="56">
+      <c r="E15" s="56" t="e">
         <f>VLOOKUP(F15,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>2</v>
+        <v>#N/A</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>2</v>
@@ -2624,7 +2625,7 @@
       </c>
       <c r="N15" s="75"/>
       <c r="O15" s="75">
-        <f>Q15/P15</f>
+        <f t="shared" si="2"/>
         <v>0.11749999999999998</v>
       </c>
       <c r="P15" s="64">
@@ -2656,11 +2657,11 @@
         <v>2.4715517241379308E-2</v>
       </c>
       <c r="X15" s="60">
-        <f>U15*Q15</f>
+        <f t="shared" si="1"/>
         <v>2.1502499999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="59" t="s">
         <v>84</v>
       </c>
@@ -2673,9 +2674,9 @@
       <c r="D16" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="E16" s="56">
+      <c r="E16" s="56" t="e">
         <f>VLOOKUP(F16,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>5</v>
+        <v>#N/A</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>8</v>
@@ -2687,7 +2688,10 @@
       </c>
       <c r="J16" s="75"/>
       <c r="K16" s="21"/>
-      <c r="L16" s="64"/>
+      <c r="L16" s="64">
+        <f>O16/I16</f>
+        <v>39.166666666666664</v>
+      </c>
       <c r="M16" s="21"/>
       <c r="N16" s="75"/>
       <c r="O16" s="75">
@@ -2723,11 +2727,11 @@
         <v>0.35817241379310344</v>
       </c>
       <c r="X16" s="60">
-        <f>U16*Q16</f>
+        <f t="shared" si="1"/>
         <v>31.161000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="59" t="s">
         <v>84</v>
       </c>
@@ -2740,9 +2744,9 @@
       <c r="D17" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="56">
+      <c r="E17" s="56" t="e">
         <f>VLOOKUP(F17,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>17</v>
+        <v>#N/A</v>
       </c>
       <c r="F17" s="14" t="s">
         <v>110</v>
@@ -2763,7 +2767,7 @@
       </c>
       <c r="N17" s="75"/>
       <c r="O17" s="75">
-        <f>Q17/P17</f>
+        <f t="shared" si="2"/>
         <v>3.5249999999999999</v>
       </c>
       <c r="P17" s="64">
@@ -2795,11 +2799,11 @@
         <v>1.3419310344827586</v>
       </c>
       <c r="X17" s="60">
-        <f>U17*Q17</f>
+        <f t="shared" si="1"/>
         <v>116.748</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" s="59" t="s">
         <v>0</v>
       </c>
@@ -2812,9 +2816,9 @@
       <c r="D18" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="56">
+      <c r="E18" s="56" t="e">
         <f>VLOOKUP(F18,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>2</v>
+        <v>#N/A</v>
       </c>
       <c r="F18" s="14" t="s">
         <v>2</v>
@@ -2840,7 +2844,7 @@
       <c r="M18" s="15"/>
       <c r="N18" s="75"/>
       <c r="O18" s="75">
-        <f>Q18/P18</f>
+        <f t="shared" si="2"/>
         <v>4.8375000000000004</v>
       </c>
       <c r="P18" s="64">
@@ -2872,11 +2876,11 @@
         <v>1.0175431034482758</v>
       </c>
       <c r="X18" s="60">
-        <f>U18*Q18</f>
+        <f t="shared" si="1"/>
         <v>88.526250000000005</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" ht="58" x14ac:dyDescent="0.35">
       <c r="A19" s="59" t="s">
         <v>0</v>
       </c>
@@ -2889,9 +2893,9 @@
       <c r="D19" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="56">
+      <c r="E19" s="56" t="e">
         <f>VLOOKUP(F19,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>2</v>
+        <v>#N/A</v>
       </c>
       <c r="F19" s="14" t="s">
         <v>2</v>
@@ -2915,7 +2919,7 @@
       <c r="M19" s="76"/>
       <c r="N19" s="75"/>
       <c r="O19" s="75">
-        <f>Q19/P19</f>
+        <f t="shared" si="2"/>
         <v>2.4187500000000002</v>
       </c>
       <c r="P19" s="64">
@@ -2947,11 +2951,11 @@
         <v>0.5087715517241379</v>
       </c>
       <c r="X19" s="60">
-        <f>U19*Q19</f>
+        <f t="shared" si="1"/>
         <v>44.263125000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="59" t="s">
         <v>0</v>
       </c>
@@ -2964,9 +2968,9 @@
       <c r="D20" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="56">
+      <c r="E20" s="56" t="e">
         <f>VLOOKUP(F20,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>7</v>
+        <v>#N/A</v>
       </c>
       <c r="F20" s="14" t="s">
         <v>13</v>
@@ -3016,14 +3020,14 @@
         <v>11.346058620689655</v>
       </c>
       <c r="X20" s="60">
-        <f>U20*Q20</f>
+        <f t="shared" si="1"/>
         <v>987.10709999999995</v>
       </c>
       <c r="Y20" s="85" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="59" t="s">
         <v>0</v>
       </c>
@@ -3036,9 +3040,9 @@
       <c r="D21" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="56">
+      <c r="E21" s="56" t="e">
         <f>VLOOKUP(F21,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>8</v>
+        <v>#N/A</v>
       </c>
       <c r="F21" s="14" t="s">
         <v>28</v>
@@ -3088,11 +3092,11 @@
         <v>0.90231034482758621</v>
       </c>
       <c r="X21" s="60">
-        <f>Q21*U21</f>
+        <f t="shared" ref="X21:X26" si="3">Q21*U21</f>
         <v>78.501000000000005</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="59" t="s">
         <v>0</v>
       </c>
@@ -3105,9 +3109,9 @@
       <c r="D22" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="56">
+      <c r="E22" s="56" t="e">
         <f>VLOOKUP(F22,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>9</v>
+        <v>#N/A</v>
       </c>
       <c r="F22" s="14" t="s">
         <v>26</v>
@@ -3157,11 +3161,11 @@
         <v>0.51240689655172411</v>
       </c>
       <c r="X22" s="60">
-        <f>Q22*U22</f>
+        <f t="shared" si="3"/>
         <v>44.5794</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="24" t="s">
         <v>38</v>
       </c>
@@ -3174,9 +3178,9 @@
       <c r="D23" s="53">
         <v>0.16</v>
       </c>
-      <c r="E23" s="56">
+      <c r="E23" s="56" t="e">
         <f>VLOOKUP(F23,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>10</v>
+        <v>#N/A</v>
       </c>
       <c r="F23" s="14" t="s">
         <v>40</v>
@@ -3226,11 +3230,11 @@
         <v>0.52668579310344821</v>
       </c>
       <c r="X23" s="60">
-        <f>Q23*U23</f>
+        <f t="shared" si="3"/>
         <v>45.821663999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="59" t="s">
         <v>17</v>
       </c>
@@ -3243,9 +3247,9 @@
       <c r="D24" s="50" t="s">
         <v>159</v>
       </c>
-      <c r="E24" s="56">
+      <c r="E24" s="56" t="e">
         <f>VLOOKUP(F24,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>11</v>
+        <v>#N/A</v>
       </c>
       <c r="F24" s="14" t="s">
         <v>14</v>
@@ -3298,11 +3302,11 @@
         <v>0.16352000000000003</v>
       </c>
       <c r="X24" s="60">
-        <f>Q24*U24</f>
+        <f t="shared" si="3"/>
         <v>14.226240000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="59" t="s">
         <v>17</v>
       </c>
@@ -3315,9 +3319,9 @@
       <c r="D25" s="50" t="s">
         <v>160</v>
       </c>
-      <c r="E25" s="56">
+      <c r="E25" s="56" t="e">
         <f>VLOOKUP(F25,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>12</v>
+        <v>#N/A</v>
       </c>
       <c r="F25" s="14" t="s">
         <v>15</v>
@@ -3370,11 +3374,11 @@
         <v>0.78839999999999999</v>
       </c>
       <c r="X25" s="60">
-        <f>Q25*U25</f>
+        <f t="shared" si="3"/>
         <v>68.590800000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="59" t="s">
         <v>17</v>
       </c>
@@ -3387,9 +3391,9 @@
       <c r="D26" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="E26" s="56">
+      <c r="E26" s="56" t="e">
         <f>VLOOKUP(F26,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>13</v>
+        <v>#N/A</v>
       </c>
       <c r="F26" s="14" t="s">
         <v>16</v>
@@ -3439,11 +3443,11 @@
         <v>0.22775999999999996</v>
       </c>
       <c r="X26" s="60">
-        <f>Q26*U26</f>
+        <f t="shared" si="3"/>
         <v>19.815119999999997</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" s="59" t="s">
         <v>18</v>
       </c>
@@ -3456,9 +3460,9 @@
       <c r="D27" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="56">
+      <c r="E27" s="56" t="e">
         <f>VLOOKUP(F27,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>2</v>
+        <v>#N/A</v>
       </c>
       <c r="F27" s="14" t="s">
         <v>2</v>
@@ -3516,11 +3520,11 @@
         <v>2.1959999999999996E-3</v>
       </c>
       <c r="X27" s="60">
-        <f>U27*Q27</f>
+        <f t="shared" ref="X27:X38" si="4">U27*Q27</f>
         <v>0.19105199999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="59" t="s">
         <v>18</v>
       </c>
@@ -3533,9 +3537,9 @@
       <c r="D28" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="56" t="str">
+      <c r="E28" s="56" t="e">
         <f>VLOOKUP(F28,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>71</v>
+        <v>#N/A</v>
       </c>
       <c r="F28" s="14" t="s">
         <v>20</v>
@@ -3593,11 +3597,11 @@
         <v>4.249439999999999</v>
       </c>
       <c r="X28" s="60">
-        <f>U28*Q28</f>
+        <f t="shared" si="4"/>
         <v>369.70127999999994</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" ht="58" x14ac:dyDescent="0.35">
       <c r="A29" s="24" t="s">
         <v>19</v>
       </c>
@@ -3610,9 +3614,9 @@
       <c r="D29" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="E29" s="56">
+      <c r="E29" s="56" t="e">
         <f>VLOOKUP(F29,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>2</v>
+        <v>#N/A</v>
       </c>
       <c r="F29" s="14" t="s">
         <v>2</v>
@@ -3674,11 +3678,11 @@
         <v>7.1517241379310356E-2</v>
       </c>
       <c r="X29" s="60">
-        <f>U29*Q29</f>
+        <f t="shared" si="4"/>
         <v>6.2220000000000004</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="59" t="s">
         <v>91</v>
       </c>
@@ -3691,9 +3695,9 @@
       <c r="D30" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E30" s="56">
+      <c r="E30" s="56" t="e">
         <f>VLOOKUP(F30,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>18</v>
+        <v>#N/A</v>
       </c>
       <c r="F30" s="14" t="s">
         <v>43</v>
@@ -3745,11 +3749,11 @@
         <v>1.4497241379310346</v>
       </c>
       <c r="X30" s="60">
-        <f>U30*Q30</f>
+        <f t="shared" si="4"/>
         <v>126.12600000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="59" t="s">
         <v>91</v>
       </c>
@@ -3762,9 +3766,9 @@
       <c r="D31" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="E31" s="56">
+      <c r="E31" s="56" t="e">
         <f>VLOOKUP(F31,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>19</v>
+        <v>#N/A</v>
       </c>
       <c r="F31" s="14" t="s">
         <v>111</v>
@@ -3818,11 +3822,11 @@
         <v>7.643819918527443E-3</v>
       </c>
       <c r="X31" s="60">
-        <f>U31*Q31</f>
+        <f t="shared" si="4"/>
         <v>0.66501233291188755</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="59" t="s">
         <v>91</v>
       </c>
@@ -3835,9 +3839,9 @@
       <c r="D32" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="56">
+      <c r="E32" s="56" t="e">
         <f>VLOOKUP(F32,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>18</v>
+        <v>#N/A</v>
       </c>
       <c r="F32" s="14" t="s">
         <v>43</v>
@@ -3891,11 +3895,11 @@
         <v>0.22772213507279673</v>
       </c>
       <c r="X32" s="60">
-        <f>U32*Q32</f>
+        <f t="shared" si="4"/>
         <v>19.811825751333316</v>
       </c>
     </row>
-    <row r="33" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="59" t="s">
         <v>45</v>
       </c>
@@ -3908,9 +3912,9 @@
       <c r="D33" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="E33" s="56">
+      <c r="E33" s="56" t="e">
         <f>VLOOKUP(F33,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>20</v>
+        <v>#N/A</v>
       </c>
       <c r="F33" s="14" t="s">
         <v>50</v>
@@ -3935,7 +3939,7 @@
         <v>7.5398223686155033E-5</v>
       </c>
       <c r="O33" s="75">
-        <f>G33*H33*I33</f>
+        <f t="shared" ref="O33:O38" si="5">G33*H33*I33</f>
         <v>1.3571680263507906E-3</v>
       </c>
       <c r="P33" s="64">
@@ -3967,11 +3971,11 @@
         <v>4.5993956424053692</v>
       </c>
       <c r="X33" s="60">
-        <f>U33*Q33</f>
+        <f t="shared" si="4"/>
         <v>400.1474208892671</v>
       </c>
     </row>
-    <row r="34" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="59" t="s">
         <v>45</v>
       </c>
@@ -3984,9 +3988,9 @@
       <c r="D34" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="E34" s="56">
+      <c r="E34" s="56" t="e">
         <f>VLOOKUP(F34,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>21</v>
+        <v>#N/A</v>
       </c>
       <c r="F34" s="14" t="s">
         <v>53</v>
@@ -4011,7 +4015,7 @@
         <v>7.5398223686155033E-5</v>
       </c>
       <c r="O34" s="75">
-        <f>G34*H34*I34</f>
+        <f t="shared" si="5"/>
         <v>1.5079644737231009E-2</v>
       </c>
       <c r="P34" s="64">
@@ -4043,11 +4047,11 @@
         <v>0.10191759891369921</v>
       </c>
       <c r="X34" s="60">
-        <f>U34*Q34</f>
+        <f t="shared" si="4"/>
         <v>8.8668311054918316</v>
       </c>
     </row>
-    <row r="35" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="59" t="s">
         <v>45</v>
       </c>
@@ -4060,9 +4064,9 @@
       <c r="D35" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="E35" s="56">
+      <c r="E35" s="56" t="e">
         <f>VLOOKUP(F35,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>21</v>
+        <v>#N/A</v>
       </c>
       <c r="F35" s="14" t="s">
         <v>53</v>
@@ -4087,7 +4091,7 @@
         <v>5.6548667764616268E-5</v>
       </c>
       <c r="O35" s="75">
-        <f>G35*H35*I35</f>
+        <f t="shared" si="5"/>
         <v>1.7530087007031044E-3</v>
       </c>
       <c r="P35" s="64">
@@ -4119,11 +4123,11 @@
         <v>1.184792087371753E-2</v>
       </c>
       <c r="X35" s="60">
-        <f>U35*Q35</f>
+        <f t="shared" si="4"/>
         <v>1.0307691160134251</v>
       </c>
     </row>
-    <row r="36" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="59" t="s">
         <v>45</v>
       </c>
@@ -4136,9 +4140,9 @@
       <c r="D36" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="E36" s="56">
+      <c r="E36" s="56" t="e">
         <f>VLOOKUP(F36,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>21</v>
+        <v>#N/A</v>
       </c>
       <c r="F36" s="14" t="s">
         <v>53</v>
@@ -4163,7 +4167,7 @@
         <v>5.0265482457436696E-4</v>
       </c>
       <c r="O36" s="75">
-        <f>G36*H36*I36</f>
+        <f t="shared" si="5"/>
         <v>1.5582299561805374E-2</v>
       </c>
       <c r="P36" s="64">
@@ -4195,11 +4199,11 @@
         <v>0.10531485221082254</v>
       </c>
       <c r="X36" s="60">
-        <f>U36*Q36</f>
+        <f t="shared" si="4"/>
         <v>9.1623921423415613</v>
       </c>
     </row>
-    <row r="37" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="59" t="s">
         <v>45</v>
       </c>
@@ -4212,9 +4216,9 @@
       <c r="D37" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="E37" s="56">
+      <c r="E37" s="56" t="e">
         <f>VLOOKUP(F37,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>20</v>
+        <v>#N/A</v>
       </c>
       <c r="F37" s="14" t="s">
         <v>50</v>
@@ -4239,7 +4243,7 @@
         <v>5.6548667764616268E-5</v>
       </c>
       <c r="O37" s="75">
-        <f>G37*H37*I37</f>
+        <f t="shared" si="5"/>
         <v>1.300619358586174E-3</v>
       </c>
       <c r="P37" s="64">
@@ -4271,11 +4275,11 @@
         <v>4.4077541573051446</v>
       </c>
       <c r="X37" s="60">
-        <f>U37*Q37</f>
+        <f t="shared" si="4"/>
         <v>383.47461168554759</v>
       </c>
     </row>
-    <row r="38" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="59" t="s">
         <v>45</v>
       </c>
@@ -4288,9 +4292,9 @@
       <c r="D38" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="E38" s="56">
+      <c r="E38" s="56" t="e">
         <f>VLOOKUP(F38,Materialen!$A$2:$B$99,2,FALSE)</f>
-        <v>20</v>
+        <v>#N/A</v>
       </c>
       <c r="F38" s="14" t="s">
         <v>50</v>
@@ -4315,7 +4319,7 @@
         <v>1.4137166941154071E-4</v>
       </c>
       <c r="O38" s="75">
-        <f>G38*H38*I38</f>
+        <f t="shared" si="5"/>
         <v>5.7019906662654756E-3</v>
       </c>
       <c r="P38" s="64">
@@ -4347,11 +4351,11 @@
         <v>19.323849747605895</v>
       </c>
       <c r="X38" s="60">
-        <f>U38*Q38</f>
+        <f t="shared" si="4"/>
         <v>1681.174928041713</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A39" s="18"/>
       <c r="B39" s="18"/>
       <c r="C39" s="18"/>
@@ -4373,7 +4377,7 @@
       <c r="S39" s="8"/>
       <c r="T39" s="82"/>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A40" s="18"/>
       <c r="B40" s="18"/>
       <c r="C40" s="18"/>
@@ -4395,7 +4399,7 @@
       <c r="S40" s="8"/>
       <c r="T40" s="82"/>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A41" s="18"/>
       <c r="B41" s="18"/>
       <c r="C41" s="18"/>
@@ -4417,7 +4421,7 @@
       <c r="S41" s="8"/>
       <c r="T41" s="82"/>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A42" s="19"/>
       <c r="B42" s="19"/>
       <c r="C42" s="19"/>
@@ -4434,7 +4438,7 @@
       <c r="O42" s="1"/>
       <c r="P42" s="72"/>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A43" s="20"/>
       <c r="B43" s="20"/>
       <c r="C43" s="20"/>
@@ -4467,26 +4471,26 @@
   <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.54296875" customWidth="1"/>
+    <col min="7" max="7" width="21.453125" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" customWidth="1"/>
+    <col min="10" max="10" width="15.26953125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="32" t="s">
         <v>70</v>
       </c>
@@ -4523,7 +4527,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
         <v>41</v>
       </c>
@@ -4564,7 +4568,7 @@
         <v>0.10555751316061705</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>29</v>
       </c>
@@ -4605,7 +4609,7 @@
         <v>7.9168134870462772E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="25" t="s">
         <v>34</v>
       </c>
@@ -4646,7 +4650,7 @@
         <v>0.70371675440411374</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
         <v>62</v>
       </c>
@@ -4687,7 +4691,7 @@
         <v>7.9168134870462772E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="25" t="s">
         <v>63</v>
       </c>
@@ -4729,7 +4733,7 @@
         <v>0.19792033717615701</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="25" t="s">
         <v>64</v>
       </c>
@@ -4753,7 +4757,7 @@
       <c r="L7" s="23"/>
       <c r="M7" s="23"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="25" t="s">
         <v>66</v>
       </c>
@@ -4777,7 +4781,7 @@
       <c r="L8" s="23"/>
       <c r="M8" s="23"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="25" t="s">
         <v>67</v>
       </c>
@@ -4801,7 +4805,7 @@
       <c r="L9" s="23"/>
       <c r="M9" s="23"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="25" t="s">
         <v>65</v>
       </c>
@@ -4825,7 +4829,7 @@
       <c r="L10" s="23"/>
       <c r="M10" s="23"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="25" t="s">
         <v>68</v>
       </c>
@@ -4849,7 +4853,7 @@
       <c r="L11" s="23"/>
       <c r="M11" s="23"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="25" t="s">
         <v>69</v>
       </c>
@@ -4872,7 +4876,7 @@
       <c r="L12" s="23"/>
       <c r="M12" s="23"/>
     </row>
-    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="25" t="s">
         <v>35</v>
       </c>
@@ -4895,7 +4899,7 @@
       <c r="L13" s="23"/>
       <c r="M13" s="23"/>
     </row>
-    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="25" t="s">
         <v>86</v>
       </c>
@@ -4918,7 +4922,7 @@
       <c r="L14" s="23"/>
       <c r="M14" s="23"/>
     </row>
-    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="25" t="s">
         <v>36</v>
       </c>
@@ -4941,7 +4945,7 @@
       <c r="L15" s="23"/>
       <c r="M15" s="23"/>
     </row>
-    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="25" t="s">
         <v>30</v>
       </c>
@@ -4967,7 +4971,7 @@
       <c r="L16" s="23"/>
       <c r="M16" s="23"/>
     </row>
-    <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
         <v>31</v>
       </c>
@@ -4993,7 +4997,7 @@
       <c r="L17" s="23"/>
       <c r="M17" s="23"/>
     </row>
-    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="21" t="s">
         <v>32</v>
       </c>
@@ -5018,7 +5022,7 @@
       <c r="L18" s="23"/>
       <c r="M18" s="23"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="30" t="s">
         <v>82</v>
       </c>
@@ -5041,7 +5045,7 @@
       <c r="L19" s="23"/>
       <c r="M19" s="23"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="21" t="s">
         <v>83</v>
       </c>
@@ -5064,7 +5068,7 @@
       <c r="L20" s="23"/>
       <c r="M20" s="23"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="21" t="s">
         <v>131</v>
       </c>
@@ -5077,7 +5081,7 @@
       <c r="D21" s="43"/>
       <c r="E21" s="26"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="86" t="s">
         <v>181</v>
       </c>
@@ -5089,7 +5093,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="23"/>
       <c r="B23" s="23"/>
       <c r="C23" s="23"/>
@@ -5099,7 +5103,7 @@
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="23"/>
       <c r="B24" s="35" t="s">
         <v>89</v>
@@ -5115,7 +5119,7 @@
       <c r="G24" s="23"/>
       <c r="H24" s="23"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="23"/>
       <c r="B25" s="68">
         <f>(0.48*0.08+0.24*0.08+0.115*0.08)</f>
@@ -5134,7 +5138,7 @@
       <c r="G25" s="23"/>
       <c r="H25" s="23"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="23"/>
       <c r="B26" s="23"/>
       <c r="C26" s="23"/>
@@ -5144,7 +5148,7 @@
       <c r="G26" s="23"/>
       <c r="H26" s="23"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D27" s="23"/>
       <c r="E27" s="23"/>
       <c r="F27" s="23"/>
@@ -5153,7 +5157,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="23"/>
       <c r="B28" s="23"/>
       <c r="C28" s="23"/>
@@ -5170,7 +5174,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="23"/>
       <c r="B29" s="23"/>
       <c r="C29" s="23"/>
@@ -5187,7 +5191,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="23"/>
       <c r="B30" s="23"/>
       <c r="C30" s="23"/>
@@ -5204,7 +5208,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="23"/>
       <c r="B31" s="23"/>
       <c r="C31" s="23"/>
@@ -5221,12 +5225,12 @@
         <v>136</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="E32" s="23"/>
       <c r="F32" s="23"/>
       <c r="G32" s="23"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="23"/>
       <c r="D33" s="23"/>
       <c r="H33" t="s">
@@ -5237,20 +5241,20 @@
         <v>2541.304347826087</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="I39" s="67"/>
       <c r="K39" s="67"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="I43" s="67"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="I47" s="67"/>
     </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I50" s="67"/>
     </row>
-    <row r="51" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I51" s="66"/>
     </row>
   </sheetData>
@@ -5268,12 +5272,12 @@
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="56.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="51" t="s">
         <v>101</v>
       </c>
@@ -5284,7 +5288,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="52" t="s">
         <v>103</v>
       </c>
@@ -5293,7 +5297,7 @@
       </c>
       <c r="C2" s="52"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="52" t="s">
         <v>104</v>
       </c>
@@ -5304,7 +5308,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="21" t="s">
         <v>106</v>
       </c>
@@ -5313,7 +5317,7 @@
       </c>
       <c r="C4" s="52"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="21" t="s">
         <v>107</v>
       </c>
@@ -5322,7 +5326,7 @@
       </c>
       <c r="C5" s="52"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="52" t="s">
         <v>112</v>
       </c>
@@ -5331,7 +5335,7 @@
       </c>
       <c r="C6" s="52"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="52" t="s">
         <v>2</v>
       </c>
@@ -5340,177 +5344,177 @@
       </c>
       <c r="C7" s="52"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="52"/>
       <c r="B8" s="52"/>
       <c r="C8" s="52"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="52"/>
       <c r="B9" s="52"/>
       <c r="C9" s="52"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="52"/>
       <c r="B10" s="52"/>
       <c r="C10" s="52"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="52"/>
       <c r="B11" s="52"/>
       <c r="C11" s="52"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="52"/>
       <c r="B12" s="52"/>
       <c r="C12" s="52"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="52"/>
       <c r="B13" s="52"/>
       <c r="C13" s="52"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="52"/>
       <c r="B14" s="52"/>
       <c r="C14" s="52"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="52"/>
       <c r="B15" s="52"/>
       <c r="C15" s="52"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="52"/>
       <c r="B16" s="52"/>
       <c r="C16" s="52"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="52"/>
       <c r="B17" s="52"/>
       <c r="C17" s="52"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="52"/>
       <c r="B18" s="52"/>
       <c r="C18" s="52"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="52"/>
       <c r="B19" s="52"/>
       <c r="C19" s="52"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="52"/>
       <c r="B20" s="52"/>
       <c r="C20" s="52"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="52"/>
       <c r="B21" s="52"/>
       <c r="C21" s="52"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="52"/>
       <c r="B22" s="52"/>
       <c r="C22" s="52"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="52"/>
       <c r="B23" s="52"/>
       <c r="C23" s="52"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="52"/>
       <c r="B24" s="52"/>
       <c r="C24" s="52"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="52"/>
       <c r="B25" s="52"/>
       <c r="C25" s="52"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="52"/>
       <c r="B26" s="52"/>
       <c r="C26" s="52"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="52"/>
       <c r="B27" s="52"/>
       <c r="C27" s="52"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="52"/>
       <c r="B28" s="52"/>
       <c r="C28" s="52"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="52"/>
       <c r="B29" s="52"/>
       <c r="C29" s="52"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="52"/>
       <c r="B30" s="52"/>
       <c r="C30" s="52"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="52"/>
       <c r="B31" s="52"/>
       <c r="C31" s="52"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="52"/>
       <c r="B32" s="52"/>
       <c r="C32" s="52"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="52"/>
       <c r="B33" s="52"/>
       <c r="C33" s="52"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="52"/>
       <c r="B34" s="52"/>
       <c r="C34" s="52"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="52"/>
       <c r="B35" s="52"/>
       <c r="C35" s="52"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="52"/>
       <c r="B36" s="52"/>
       <c r="C36" s="52"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="52"/>
       <c r="B37" s="52"/>
       <c r="C37" s="52"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="52"/>
       <c r="B38" s="52"/>
       <c r="C38" s="52"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="52"/>
       <c r="B39" s="52"/>
       <c r="C39" s="52"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="52"/>
       <c r="B40" s="52"/>
       <c r="C40" s="52"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="52"/>
       <c r="B41" s="52"/>
       <c r="C41" s="52"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="52"/>
       <c r="B42" s="52"/>
       <c r="C42" s="52"/>
@@ -5528,1000 +5532,1000 @@
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" style="57" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" style="57" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="str">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="e">
         <f>[1]!Bouwmaterialen[[#Headers],[Bouwmateriaal]]</f>
-        <v>Bouwmateriaal</v>
-      </c>
-      <c r="B1" s="57" t="str">
+        <v>#REF!</v>
+      </c>
+      <c r="B1" s="57" t="e">
         <f>[1]!Bouwmaterialen[[#Headers],[Key bouwmateriaal]]</f>
-        <v>Key bouwmateriaal</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Baksteen</v>
-      </c>
-      <c r="B2" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Hout</v>
-      </c>
-      <c r="B3" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Kalkzandsteen</v>
-      </c>
-      <c r="B4" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Vulpanelen van hout of asbest</v>
-      </c>
-      <c r="B5" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Polystyreen</v>
-      </c>
-      <c r="B6" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Stucwerk</v>
-      </c>
-      <c r="B7" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>OSB + PUR</v>
-      </c>
-      <c r="B8" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Keramisch</v>
-      </c>
-      <c r="B9" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Beton</v>
-      </c>
-      <c r="B10" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Glaswol</v>
-      </c>
-      <c r="B11" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Enkelglas</v>
-      </c>
-      <c r="B12" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Dubbelglas</v>
-      </c>
-      <c r="B13" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>HR-glas</v>
-      </c>
-      <c r="B14" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>RVS</v>
-      </c>
-      <c r="B15" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Schelpkalkmortel</v>
-      </c>
-      <c r="B16" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Gipsplaat</v>
-      </c>
-      <c r="B17" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Gasbeton</v>
-      </c>
-      <c r="B18" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Zink</v>
-      </c>
-      <c r="B19" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>PVC</v>
-      </c>
-      <c r="B20" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Koper</v>
-      </c>
-      <c r="B21" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Kunststof</v>
-      </c>
-      <c r="B22" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>ZOAB</v>
-      </c>
-      <c r="B23" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Triplex</v>
-      </c>
-      <c r="B24" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Betonpuin</v>
-      </c>
-      <c r="B25" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Metselwerkpuin</v>
-      </c>
-      <c r="B26" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Asfaltpuin</v>
-      </c>
-      <c r="B27" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Mengpuin</v>
-      </c>
-      <c r="B28" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Zinkrecycling</v>
-      </c>
-      <c r="B29" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Gipshoudend materiaal</v>
-      </c>
-      <c r="B30" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>RVS-recycling</v>
-      </c>
-      <c r="B31" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>A-hout (onbehandeld)</v>
-      </c>
-      <c r="B32" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>B-hout (behandeld)</v>
-      </c>
-      <c r="B33" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>C-hout (geïmpregneerd)</v>
-      </c>
-      <c r="B34" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Non-ferromagnetische metalen</v>
-      </c>
-      <c r="B35" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Ferromagnetische metalen</v>
-      </c>
-      <c r="B36" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Glasrecycling</v>
-      </c>
-      <c r="B37" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Tapijtafval</v>
-      </c>
-      <c r="B38" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Kunststoffenverwerking</v>
-      </c>
-      <c r="B39" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Isolatiemateriaalafval</v>
-      </c>
-      <c r="B40" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Dakbedekkingsmateriaal bitumineus</v>
-      </c>
-      <c r="B41" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Plafondplatenafval</v>
-      </c>
-      <c r="B42" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Asbesthoudend afval</v>
-      </c>
-      <c r="B43" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Gemengd bouw- en sloopafval</v>
-      </c>
-      <c r="B44" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Multiplex</v>
-      </c>
-      <c r="B45" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Bitumineuze laag</v>
-      </c>
-      <c r="B46" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Grind</v>
-      </c>
-      <c r="B47" s="57">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Gewapend beton</v>
-      </c>
-      <c r="B48" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Aluminium</v>
-      </c>
-      <c r="B49" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Plafondplaat</v>
-      </c>
-      <c r="B50" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Rubber</v>
-      </c>
-      <c r="B51" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>AC Base</v>
-      </c>
-      <c r="B52" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>51</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>AC Surf</v>
-      </c>
-      <c r="B53" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Klinkers (rood)</v>
-      </c>
-      <c r="B54" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Menggranulaat</v>
-      </c>
-      <c r="B55" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Menggranulaat of licht gebonden fundering</v>
-      </c>
-      <c r="B56" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Zand</v>
-      </c>
-      <c r="B57" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Zandcement</v>
-      </c>
-      <c r="B58" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>57</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Stoeptegels (beton)</v>
-      </c>
-      <c r="B59" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Groenbedekking</v>
-      </c>
-      <c r="B60" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>59</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>GFT</v>
-      </c>
-      <c r="B61" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Betonklinkers</v>
-      </c>
-      <c r="B62" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>61</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Natuursteen</v>
-      </c>
-      <c r="B63" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>62</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Sandwichpanelen</v>
-      </c>
-      <c r="B64" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Trespa</v>
-      </c>
-      <c r="B65" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Isolatiemateriaal</v>
-      </c>
-      <c r="B66" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>65</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Tapijt</v>
-      </c>
-      <c r="B67" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>66</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Steenwolplaten</v>
-      </c>
-      <c r="B68" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>67</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Koperrecycling</v>
-      </c>
-      <c r="B69" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>68</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Aluminiumrecycling</v>
-      </c>
-      <c r="B70" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>69</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Staalrecycling (niet roestvrij)</v>
-      </c>
-      <c r="B71" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Staal</v>
-      </c>
-      <c r="B72" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>71</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Betonasfalt</v>
-      </c>
-      <c r="B73" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>72</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>PV monokristallijn (24,72 kg/m2)</v>
-      </c>
-      <c r="B74" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>73</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>PV polykristallijn (24,72 kg/m2)</v>
-      </c>
-      <c r="B75" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>74</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Electronica (voor regeleenheden)</v>
-      </c>
-      <c r="B76" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>Electronisch afval (ook PV)</v>
-      </c>
-      <c r="B77" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>76</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>geen</v>
-      </c>
-      <c r="B78" s="57" t="str">
-        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>99</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B2" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B3" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B4" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B5" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B6" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B7" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B8" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B9" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B10" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B11" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B12" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B13" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B14" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B15" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B16" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B17" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B18" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B19" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B20" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B21" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B22" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B23" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B24" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B25" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B26" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B27" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B28" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B29" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B30" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B31" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B32" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B33" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B34" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B35" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B36" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B37" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B38" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B39" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B40" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B41" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B42" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B43" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B44" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B45" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B46" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B47" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B48" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B49" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B50" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B51" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B52" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B53" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B54" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B55" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B56" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B57" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B58" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B59" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B60" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B61" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B62" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B63" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B64" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B65" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B66" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B67" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B68" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B69" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B70" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B71" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B72" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B73" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B74" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B75" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B76" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B77" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B78" s="57" t="e">
+        <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="B79" s="57" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="B80" s="57" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="B81" s="57" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="B82" s="57" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="B83" s="57" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="B84" s="57" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="B85" s="57" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="B86" s="57" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="B87" s="57" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="B88" s="57" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="B89" s="57" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="B90" s="57" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="B91" s="57" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="B92" s="57" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="B93" s="57" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="B94" s="57" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="B95" s="57" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="B96" s="57" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="B97" s="57" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="B98" s="57" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Bouwmateriaal]]</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="B99" s="57" t="e">
         <f>[1]!Bouwmaterialen[[#This Row],[Key bouwmateriaal]]</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
     </row>
   </sheetData>
@@ -6530,6 +6534,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100064BEAEE4B1CA04CBF3B3E77AAD1867B" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fe5e8bff33f492ae91bd2ecdf8a74c45">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="815ba399-014b-4508-8f04-2125e654312d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b92c3777d5d0f0d563bb22ddfaee4d91" ns3:_="">
     <xsd:import namespace="815ba399-014b-4508-8f04-2125e654312d"/>
@@ -6693,12 +6703,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -6709,6 +6713,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F066166-6AE1-43C4-B122-965363BDD2A0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="815ba399-014b-4508-8f04-2125e654312d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55B69CDE-BD68-47ED-B0B5-54B1C1ADAAC7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6726,22 +6746,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F066166-6AE1-43C4-B122-965363BDD2A0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="815ba399-014b-4508-8f04-2125e654312d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{731318B2-9C1F-4072-98B1-5D72029F1F67}">
   <ds:schemaRefs>

</xml_diff>